<commit_message>
Use Straight-Thru Ethernet calble for coincidence connection
</commit_message>
<xml_diff>
--- a/Purchasing_List_v3X_sa.xlsx
+++ b/Purchasing_List_v3X_sa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saxani/My Drive/CosmicWatch/GitHub/CosmicWatch-Desktop-Muon-Detector-v3X/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF3FAEE-58AE-E74A-8D88-D24B2134C04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499AFB46-B51B-C149-88BB-E88B03FC28A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,9 +637,6 @@
     <t>Total cost:</t>
   </si>
   <si>
-    <t>0.5 ft (or longer) CAT6 Cable</t>
-  </si>
-  <si>
     <t>BNC cable for testing (optional)</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>Digikey Part Number: RNCP0805FTD10K0DKR</t>
+  </si>
+  <si>
+    <t>0.5 ft (or longer) CAT6 Cable (STRAIGHT-Thru ONLY)</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="88" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1613,7 +1613,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F10" s="36">
         <v>0.1</v>
@@ -1647,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F11" s="36">
         <v>0.1</v>
@@ -1681,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="36">
         <v>0.1</v>
@@ -1715,7 +1715,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F13" s="36">
         <v>0.1</v>
@@ -1749,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F14" s="36">
         <v>0.1</v>
@@ -1777,13 +1777,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D15" s="35">
         <v>1</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F15" s="36">
         <v>0.1</v>
@@ -1800,10 +1800,10 @@
         <v>2.7000000000000003E-2</v>
       </c>
       <c r="J15" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="K15" s="38" t="s">
         <v>247</v>
-      </c>
-      <c r="K15" s="38" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1817,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F16" s="36">
         <v>0.14000000000000001</v>
@@ -1851,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F17" s="36">
         <v>0.1</v>
@@ -1885,7 +1885,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F18" s="36">
         <v>0.1</v>
@@ -1919,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F19" s="36">
         <v>0.1</v>
@@ -1953,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F20" s="36">
         <v>0.1</v>
@@ -1987,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F21" s="36">
         <v>0.13</v>
@@ -2021,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F22" s="36">
         <v>0.11</v>
@@ -2055,7 +2055,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F23" s="36">
         <v>0.19</v>
@@ -2089,7 +2089,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F24" s="36">
         <v>0.11</v>
@@ -2123,7 +2123,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F25" s="36">
         <v>0.08</v>
@@ -2157,7 +2157,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F26" s="36">
         <v>0.1</v>
@@ -2191,7 +2191,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F27" s="36">
         <v>0.11</v>
@@ -2225,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F28" s="36">
         <v>0.08</v>
@@ -2259,7 +2259,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F29" s="36">
         <v>0.1</v>
@@ -2293,7 +2293,7 @@
         <v>75</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F30" s="36">
         <v>1.04</v>
@@ -2327,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F31" s="36">
         <v>4</v>
@@ -2362,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F32" s="36">
         <v>0.15</v>
@@ -2397,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F33" s="36">
         <v>0.1</v>
@@ -2431,7 +2431,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F34" s="36">
         <v>1.92</v>
@@ -2466,7 +2466,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F35" s="36">
         <v>1.67</v>
@@ -2501,7 +2501,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F36" s="36">
         <v>0.13</v>
@@ -2535,7 +2535,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F37" s="36">
         <v>0.89</v>
@@ -2570,7 +2570,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F38" s="36">
         <v>0.13</v>
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F39" s="36">
         <v>2.48</v>
@@ -2642,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F40" s="36">
         <v>0.33</v>
@@ -2679,7 +2679,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F41" s="36">
         <v>0.53</v>
@@ -2714,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F42" s="36">
         <v>28.41</v>
@@ -2743,13 +2743,13 @@
         <v>28</v>
       </c>
       <c r="C43" s="67" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D43" s="68">
         <v>1</v>
       </c>
       <c r="E43" s="68" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F43" s="69">
         <v>0.45</v>
@@ -2788,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="48" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F44" s="49">
         <f>6.89/10</f>
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F45" s="49">
         <f>7.39/5</f>
@@ -2866,7 +2866,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F46" s="49">
         <v>6.99</v>
@@ -2902,7 +2902,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F47" s="49">
         <f t="shared" ref="F47:F48" si="7">6.99/100</f>
@@ -2938,7 +2938,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F48" s="49">
         <f t="shared" si="7"/>
@@ -2975,7 +2975,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F49" s="49">
         <v>5</v>
@@ -3013,7 +3013,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="48" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F50" s="49">
         <f>7.29/6</f>
@@ -3086,7 +3086,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F52" s="49">
         <v>1.69</v>
@@ -3120,7 +3120,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F53" s="49">
         <v>2.6</v>
@@ -3171,8 +3171,8 @@
         <f t="shared" si="9"/>
         <v>0.88900000000000001</v>
       </c>
-      <c r="J54" s="52" t="s">
-        <v>196</v>
+      <c r="J54" s="50" t="s">
+        <v>248</v>
       </c>
       <c r="K54" s="55" t="s">
         <v>193</v>
@@ -3184,7 +3184,7 @@
         <v>35</v>
       </c>
       <c r="C55" s="53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D55" s="48">
         <v>1</v>
@@ -3224,7 +3224,7 @@
         <v>2</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F56" s="44">
         <v>0.7</v>
@@ -3252,7 +3252,7 @@
         <v>31</v>
       </c>
       <c r="C57" s="42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D57" s="43">
         <v>4</v>
@@ -3293,7 +3293,7 @@
         <v>4</v>
       </c>
       <c r="E58" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F58" s="44">
         <f>2.65/100</f>
@@ -3363,7 +3363,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="58" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F60" s="59">
         <v>0.99</v>

</xml_diff>